<commit_message>
Done Chapter 4 "Getting Connected: A Trip to Webville"
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F269E238-6EAF-4F0B-9FD0-E6570396E90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7627DBC8-6AFC-44CA-97AE-EFA8E5266957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12852" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
+    <sheet name="4. Getting Connected A Trip to " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="179">
   <si>
     <t>Label</t>
   </si>
@@ -507,6 +508,69 @@
   </si>
   <si>
     <t>Neither</t>
+  </si>
+  <si>
+    <t>ACROSS</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>A Mac FTP App</t>
+  </si>
+  <si>
+    <t>Unique name on the Web</t>
+  </si>
+  <si>
+    <t>The file you get when you ask for a directory</t>
+  </si>
+  <si>
+    <t>What are you supposed to send back from Webville?</t>
+  </si>
+  <si>
+    <t>Top Directory of your Website</t>
+  </si>
+  <si>
+    <t>Request/Response protocol</t>
+  </si>
+  <si>
+    <t>Keep your link labels _____</t>
+  </si>
+  <si>
+    <t>Attribute used to make an element into a destination</t>
+  </si>
+  <si>
+    <t>Earl sold these</t>
+  </si>
+  <si>
+    <t>Web Address to a resource</t>
+  </si>
+  <si>
+    <t>Top directory of your website</t>
+  </si>
+  <si>
+    <t>Protocol we've been using up until this Chapter</t>
+  </si>
+  <si>
+    <t>People can scan these rather than reading text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path from the root </t>
+  </si>
+  <si>
+    <t>Control domain names</t>
+  </si>
+  <si>
+    <t>Always use these kind of links when linking to pages on same server</t>
+  </si>
+  <si>
+    <t>Wrong way to pronounce URL</t>
+  </si>
+  <si>
+    <t>Informative caffeine site</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -565,7 +629,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +651,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -849,9 +919,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -875,6 +942,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1158,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X100" sqref="X100"/>
+    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,7 +1243,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>148</v>
       </c>
     </row>
@@ -1242,10 +1314,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="29"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
@@ -1316,39 +1388,39 @@
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="30"/>
-    </row>
-    <row r="19" spans="1:28" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+    </row>
+    <row r="19" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="I20" s="5"/>
@@ -1941,10 +2013,10 @@
       <c r="M37" s="3"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B38" s="33"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -2077,10 +2149,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="32"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
@@ -2096,12 +2168,12 @@
       <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
     </row>
     <row r="58" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
@@ -2284,16 +2356,16 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="34"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
+      <c r="A71" s="33"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="29"/>
+      <c r="B73" s="28"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -2351,10 +2423,10 @@
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="B87" s="30"/>
+      <c r="B87" s="29"/>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="I88" s="2">
@@ -2363,155 +2435,155 @@
       <c r="J88" s="2">
         <v>2</v>
       </c>
-      <c r="K88" s="37" t="s">
+      <c r="K88" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="L88" s="45" t="s">
+      <c r="L88" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="M88" s="38" t="s">
+      <c r="M88" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="N88" s="36"/>
-      <c r="O88" s="36"/>
-      <c r="P88" s="36"/>
-      <c r="Q88" s="36"/>
-      <c r="R88" s="36"/>
-      <c r="S88" s="36"/>
-      <c r="T88" s="36"/>
-      <c r="U88" s="36"/>
-      <c r="V88" s="36"/>
-      <c r="W88" s="36"/>
-      <c r="X88" s="36"/>
-      <c r="Y88" s="45" t="s">
+      <c r="N88" s="35"/>
+      <c r="O88" s="35"/>
+      <c r="P88" s="35"/>
+      <c r="Q88" s="35"/>
+      <c r="R88" s="35"/>
+      <c r="S88" s="35"/>
+      <c r="T88" s="35"/>
+      <c r="U88" s="35"/>
+      <c r="V88" s="35"/>
+      <c r="W88" s="35"/>
+      <c r="X88" s="35"/>
+      <c r="Y88" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="Z88" s="36"/>
-      <c r="AA88" s="36"/>
-      <c r="AB88" s="36"/>
+      <c r="Z88" s="35"/>
+      <c r="AA88" s="35"/>
+      <c r="AB88" s="35"/>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I89" s="36"/>
-      <c r="J89" s="36"/>
-      <c r="K89" s="36"/>
-      <c r="L89" s="46" t="s">
+      <c r="I89" s="35"/>
+      <c r="J89" s="35"/>
+      <c r="K89" s="35"/>
+      <c r="L89" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="M89" s="36"/>
-      <c r="N89" s="36"/>
+      <c r="M89" s="35"/>
+      <c r="N89" s="35"/>
       <c r="O89" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P89" s="36"/>
-      <c r="Q89" s="36"/>
-      <c r="R89" s="36"/>
-      <c r="S89" s="36"/>
-      <c r="T89" s="39" t="s">
+      <c r="P89" s="35"/>
+      <c r="Q89" s="35"/>
+      <c r="R89" s="35"/>
+      <c r="S89" s="35"/>
+      <c r="T89" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="U89" s="36"/>
-      <c r="V89" s="36"/>
-      <c r="W89" s="36"/>
-      <c r="X89" s="36"/>
-      <c r="Y89" s="46" t="s">
+      <c r="U89" s="35"/>
+      <c r="V89" s="35"/>
+      <c r="W89" s="35"/>
+      <c r="X89" s="35"/>
+      <c r="Y89" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="Z89" s="36"/>
-      <c r="AA89" s="36"/>
-      <c r="AB89" s="36"/>
+      <c r="Z89" s="35"/>
+      <c r="AA89" s="35"/>
+      <c r="AB89" s="35"/>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I90" s="36"/>
+      <c r="I90" s="35"/>
       <c r="J90" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L90" s="45" t="s">
+      <c r="L90" s="44" t="s">
         <v>44</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N90" s="37" t="s">
+      <c r="N90" s="36" t="s">
         <v>46</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="P90" s="38" t="s">
+      <c r="P90" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="Q90" s="36"/>
+      <c r="Q90" s="35"/>
       <c r="R90" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S90" s="36"/>
+      <c r="S90" s="35"/>
       <c r="T90" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="U90" s="36"/>
+      <c r="U90" s="35"/>
       <c r="V90" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="W90" s="36"/>
-      <c r="X90" s="36"/>
-      <c r="Y90" s="45" t="s">
+      <c r="W90" s="35"/>
+      <c r="X90" s="35"/>
+      <c r="Y90" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="Z90" s="36"/>
-      <c r="AA90" s="36"/>
-      <c r="AB90" s="36"/>
+      <c r="Z90" s="35"/>
+      <c r="AA90" s="35"/>
+      <c r="AB90" s="35"/>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I91" s="36"/>
-      <c r="J91" s="36"/>
-      <c r="K91" s="36"/>
-      <c r="L91" s="47" t="s">
+      <c r="I91" s="35"/>
+      <c r="J91" s="35"/>
+      <c r="K91" s="35"/>
+      <c r="L91" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="M91" s="36"/>
-      <c r="N91" s="36"/>
-      <c r="O91" s="39" t="s">
+      <c r="M91" s="35"/>
+      <c r="N91" s="35"/>
+      <c r="O91" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="P91" s="36"/>
-      <c r="Q91" s="36"/>
+      <c r="P91" s="35"/>
+      <c r="Q91" s="35"/>
       <c r="R91" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S91" s="36"/>
-      <c r="T91" s="41" t="s">
+      <c r="S91" s="35"/>
+      <c r="T91" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="U91" s="41" t="s">
+      <c r="U91" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="V91" s="41" t="s">
+      <c r="V91" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="W91" s="41" t="s">
+      <c r="W91" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="X91" s="41" t="s">
+      <c r="X91" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="Y91" s="45" t="s">
+      <c r="Y91" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="Z91" s="36"/>
-      <c r="AA91" s="36"/>
-      <c r="AB91" s="36"/>
+      <c r="Z91" s="35"/>
+      <c r="AA91" s="35"/>
+      <c r="AB91" s="35"/>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I92" s="36"/>
-      <c r="J92" s="36"/>
-      <c r="K92" s="36"/>
-      <c r="L92" s="45" t="s">
+      <c r="I92" s="35"/>
+      <c r="J92" s="35"/>
+      <c r="K92" s="35"/>
+      <c r="L92" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="M92" s="36"/>
+      <c r="M92" s="35"/>
       <c r="N92" s="2" t="s">
         <v>55</v>
       </c>
@@ -2521,77 +2593,77 @@
       <c r="P92" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Q92" s="37" t="s">
+      <c r="Q92" s="36" t="s">
         <v>43</v>
       </c>
       <c r="R92" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S92" s="38" t="s">
+      <c r="S92" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="T92" s="40" t="s">
+      <c r="T92" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="U92" s="36"/>
-      <c r="V92" s="40" t="s">
+      <c r="U92" s="35"/>
+      <c r="V92" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="W92" s="36"/>
-      <c r="X92" s="36"/>
-      <c r="Y92" s="45" t="s">
+      <c r="W92" s="35"/>
+      <c r="X92" s="35"/>
+      <c r="Y92" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="Z92" s="36"/>
-      <c r="AA92" s="36"/>
-      <c r="AB92" s="36"/>
+      <c r="Z92" s="35"/>
+      <c r="AA92" s="35"/>
+      <c r="AB92" s="35"/>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I93" s="36"/>
-      <c r="J93" s="45" t="s">
+      <c r="I93" s="35"/>
+      <c r="J93" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="K93" s="36"/>
-      <c r="L93" s="46" t="s">
+      <c r="K93" s="35"/>
+      <c r="L93" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="M93" s="36"/>
-      <c r="N93" s="36"/>
-      <c r="O93" s="42" t="s">
+      <c r="M93" s="35"/>
+      <c r="N93" s="35"/>
+      <c r="O93" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="P93" s="36"/>
-      <c r="Q93" s="36"/>
-      <c r="R93" s="39" t="s">
+      <c r="P93" s="35"/>
+      <c r="Q93" s="35"/>
+      <c r="R93" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="S93" s="36"/>
-      <c r="T93" s="36"/>
-      <c r="U93" s="36"/>
+      <c r="S93" s="35"/>
+      <c r="T93" s="35"/>
+      <c r="U93" s="35"/>
       <c r="V93" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="W93" s="36"/>
+      <c r="W93" s="35"/>
       <c r="X93" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Y93" s="36"/>
-      <c r="Z93" s="36"/>
-      <c r="AA93" s="36"/>
-      <c r="AB93" s="36"/>
+      <c r="Y93" s="35"/>
+      <c r="Z93" s="35"/>
+      <c r="AA93" s="35"/>
+      <c r="AB93" s="35"/>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I94" s="36"/>
-      <c r="J94" s="45" t="s">
+      <c r="I94" s="35"/>
+      <c r="J94" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="K94" s="38" t="s">
+      <c r="K94" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="L94" s="45" t="s">
+      <c r="L94" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="M94" s="36"/>
+      <c r="M94" s="35"/>
       <c r="N94" s="2" t="s">
         <v>44</v>
       </c>
@@ -2610,279 +2682,279 @@
       <c r="S94" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="T94" s="36"/>
-      <c r="U94" s="36"/>
+      <c r="T94" s="35"/>
+      <c r="U94" s="35"/>
       <c r="V94" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="W94" s="36"/>
+      <c r="W94" s="35"/>
       <c r="X94" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Y94" s="36"/>
-      <c r="Z94" s="36"/>
-      <c r="AA94" s="36"/>
-      <c r="AB94" s="36"/>
+      <c r="Y94" s="35"/>
+      <c r="Z94" s="35"/>
+      <c r="AA94" s="35"/>
+      <c r="AB94" s="35"/>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I95" s="36"/>
-      <c r="J95" s="45" t="s">
+      <c r="I95" s="35"/>
+      <c r="J95" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="K95" s="36"/>
-      <c r="L95" s="36"/>
-      <c r="M95" s="36"/>
-      <c r="N95" s="36"/>
-      <c r="O95" s="40" t="s">
+      <c r="K95" s="35"/>
+      <c r="L95" s="35"/>
+      <c r="M95" s="35"/>
+      <c r="N95" s="35"/>
+      <c r="O95" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="P95" s="36"/>
-      <c r="Q95" s="36"/>
-      <c r="R95" s="40" t="s">
+      <c r="P95" s="35"/>
+      <c r="Q95" s="35"/>
+      <c r="R95" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="S95" s="36"/>
-      <c r="T95" s="36"/>
-      <c r="U95" s="36"/>
+      <c r="S95" s="35"/>
+      <c r="T95" s="35"/>
+      <c r="U95" s="35"/>
       <c r="V95" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="W95" s="36"/>
+      <c r="W95" s="35"/>
       <c r="X95" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Y95" s="36"/>
-      <c r="Z95" s="36"/>
-      <c r="AA95" s="36"/>
-      <c r="AB95" s="36"/>
+      <c r="Y95" s="35"/>
+      <c r="Z95" s="35"/>
+      <c r="AA95" s="35"/>
+      <c r="AB95" s="35"/>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I96" s="36"/>
-      <c r="J96" s="45" t="s">
+      <c r="I96" s="35"/>
+      <c r="J96" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="K96" s="36"/>
-      <c r="L96" s="36"/>
-      <c r="M96" s="36"/>
-      <c r="N96" s="36"/>
+      <c r="K96" s="35"/>
+      <c r="L96" s="35"/>
+      <c r="M96" s="35"/>
+      <c r="N96" s="35"/>
       <c r="O96" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P96" s="36"/>
-      <c r="Q96" s="36"/>
+      <c r="P96" s="35"/>
+      <c r="Q96" s="35"/>
       <c r="R96" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S96" s="36"/>
-      <c r="T96" s="36"/>
-      <c r="U96" s="36"/>
+      <c r="S96" s="35"/>
+      <c r="T96" s="35"/>
+      <c r="U96" s="35"/>
       <c r="V96" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="W96" s="36"/>
+      <c r="W96" s="35"/>
       <c r="X96" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Y96" s="36"/>
-      <c r="Z96" s="36"/>
-      <c r="AA96" s="36"/>
-      <c r="AB96" s="36"/>
+      <c r="Y96" s="35"/>
+      <c r="Z96" s="35"/>
+      <c r="AA96" s="35"/>
+      <c r="AB96" s="35"/>
     </row>
     <row r="97" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I97" s="36"/>
-      <c r="J97" s="45" t="s">
+      <c r="I97" s="35"/>
+      <c r="J97" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="K97" s="36"/>
-      <c r="L97" s="36"/>
-      <c r="M97" s="36"/>
-      <c r="N97" s="36"/>
+      <c r="K97" s="35"/>
+      <c r="L97" s="35"/>
+      <c r="M97" s="35"/>
+      <c r="N97" s="35"/>
       <c r="O97" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P97" s="36"/>
-      <c r="Q97" s="36"/>
+      <c r="P97" s="35"/>
+      <c r="Q97" s="35"/>
       <c r="R97" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S97" s="36"/>
-      <c r="T97" s="36"/>
-      <c r="U97" s="36"/>
+      <c r="S97" s="35"/>
+      <c r="T97" s="35"/>
+      <c r="U97" s="35"/>
       <c r="V97" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="W97" s="36"/>
+      <c r="W97" s="35"/>
       <c r="X97" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y97" s="36"/>
-      <c r="Z97" s="36"/>
-      <c r="AA97" s="36"/>
-      <c r="AB97" s="36"/>
+      <c r="Y97" s="35"/>
+      <c r="Z97" s="35"/>
+      <c r="AA97" s="35"/>
+      <c r="AB97" s="35"/>
     </row>
     <row r="98" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I98" s="36"/>
-      <c r="J98" s="36"/>
-      <c r="K98" s="36"/>
-      <c r="L98" s="36"/>
-      <c r="M98" s="36"/>
-      <c r="N98" s="36"/>
-      <c r="O98" s="36"/>
-      <c r="P98" s="36"/>
-      <c r="Q98" s="36"/>
-      <c r="R98" s="39" t="s">
+      <c r="I98" s="35"/>
+      <c r="J98" s="35"/>
+      <c r="K98" s="35"/>
+      <c r="L98" s="35"/>
+      <c r="M98" s="35"/>
+      <c r="N98" s="35"/>
+      <c r="O98" s="35"/>
+      <c r="P98" s="35"/>
+      <c r="Q98" s="35"/>
+      <c r="R98" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="S98" s="36"/>
-      <c r="T98" s="36"/>
-      <c r="U98" s="36"/>
+      <c r="S98" s="35"/>
+      <c r="T98" s="35"/>
+      <c r="U98" s="35"/>
       <c r="V98" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="W98" s="36"/>
+      <c r="W98" s="35"/>
       <c r="X98" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Y98" s="36"/>
-      <c r="Z98" s="36"/>
-      <c r="AA98" s="36"/>
-      <c r="AB98" s="36"/>
+      <c r="Y98" s="35"/>
+      <c r="Z98" s="35"/>
+      <c r="AA98" s="35"/>
+      <c r="AB98" s="35"/>
     </row>
     <row r="99" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
-      <c r="K99" s="36"/>
-      <c r="L99" s="36"/>
+      <c r="I99" s="35"/>
+      <c r="J99" s="35"/>
+      <c r="K99" s="35"/>
+      <c r="L99" s="35"/>
       <c r="M99" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N99" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O99" s="41" t="s">
+      <c r="O99" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="P99" s="41" t="s">
+      <c r="P99" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="Q99" s="41" t="s">
+      <c r="Q99" s="40" t="s">
         <v>40</v>
       </c>
       <c r="R99" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S99" s="41" t="s">
+      <c r="S99" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="T99" s="41" t="s">
+      <c r="T99" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="U99" s="41" t="s">
+      <c r="U99" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="V99" s="41" t="s">
+      <c r="V99" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="W99" s="43" t="s">
+      <c r="W99" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="X99" s="41" t="s">
+      <c r="X99" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="Y99" s="44" t="s">
+      <c r="Y99" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="Z99" s="36"/>
-      <c r="AA99" s="36"/>
-      <c r="AB99" s="36"/>
+      <c r="Z99" s="35"/>
+      <c r="AA99" s="35"/>
+      <c r="AB99" s="35"/>
     </row>
     <row r="100" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
-      <c r="K100" s="36"/>
-      <c r="L100" s="36"/>
-      <c r="M100" s="36"/>
-      <c r="N100" s="36"/>
-      <c r="O100" s="36"/>
-      <c r="P100" s="36"/>
-      <c r="Q100" s="36"/>
-      <c r="R100" s="36"/>
-      <c r="S100" s="36"/>
-      <c r="T100" s="36"/>
-      <c r="U100" s="36"/>
-      <c r="V100" s="36"/>
-      <c r="W100" s="36"/>
-      <c r="X100" s="36"/>
-      <c r="Y100" s="36"/>
-      <c r="Z100" s="36"/>
-      <c r="AA100" s="36"/>
-      <c r="AB100" s="36"/>
+      <c r="I100" s="35"/>
+      <c r="J100" s="35"/>
+      <c r="K100" s="35"/>
+      <c r="L100" s="35"/>
+      <c r="M100" s="35"/>
+      <c r="N100" s="35"/>
+      <c r="O100" s="35"/>
+      <c r="P100" s="35"/>
+      <c r="Q100" s="35"/>
+      <c r="R100" s="35"/>
+      <c r="S100" s="35"/>
+      <c r="T100" s="35"/>
+      <c r="U100" s="35"/>
+      <c r="V100" s="35"/>
+      <c r="W100" s="35"/>
+      <c r="X100" s="35"/>
+      <c r="Y100" s="35"/>
+      <c r="Z100" s="35"/>
+      <c r="AA100" s="35"/>
+      <c r="AB100" s="35"/>
     </row>
     <row r="101" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
-      <c r="K101" s="36"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="36"/>
-      <c r="N101" s="36"/>
-      <c r="O101" s="36"/>
-      <c r="P101" s="36"/>
-      <c r="Q101" s="36"/>
-      <c r="R101" s="36"/>
-      <c r="S101" s="36"/>
-      <c r="T101" s="36"/>
-      <c r="U101" s="36"/>
-      <c r="V101" s="36"/>
-      <c r="W101" s="36"/>
-      <c r="X101" s="36"/>
-      <c r="Y101" s="36"/>
-      <c r="Z101" s="36"/>
-      <c r="AA101" s="36"/>
-      <c r="AB101" s="36"/>
+      <c r="I101" s="35"/>
+      <c r="J101" s="35"/>
+      <c r="K101" s="35"/>
+      <c r="L101" s="35"/>
+      <c r="M101" s="35"/>
+      <c r="N101" s="35"/>
+      <c r="O101" s="35"/>
+      <c r="P101" s="35"/>
+      <c r="Q101" s="35"/>
+      <c r="R101" s="35"/>
+      <c r="S101" s="35"/>
+      <c r="T101" s="35"/>
+      <c r="U101" s="35"/>
+      <c r="V101" s="35"/>
+      <c r="W101" s="35"/>
+      <c r="X101" s="35"/>
+      <c r="Y101" s="35"/>
+      <c r="Z101" s="35"/>
+      <c r="AA101" s="35"/>
+      <c r="AB101" s="35"/>
     </row>
     <row r="102" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
-      <c r="K102" s="36"/>
-      <c r="L102" s="36"/>
-      <c r="M102" s="36"/>
-      <c r="N102" s="36"/>
-      <c r="O102" s="36"/>
-      <c r="P102" s="36"/>
-      <c r="Q102" s="36"/>
-      <c r="R102" s="36"/>
-      <c r="S102" s="36"/>
-      <c r="T102" s="36"/>
-      <c r="U102" s="36"/>
-      <c r="V102" s="36"/>
-      <c r="W102" s="36"/>
-      <c r="X102" s="36"/>
-      <c r="Y102" s="36"/>
-      <c r="Z102" s="36"/>
-      <c r="AA102" s="36"/>
-      <c r="AB102" s="36"/>
+      <c r="I102" s="35"/>
+      <c r="J102" s="35"/>
+      <c r="K102" s="35"/>
+      <c r="L102" s="35"/>
+      <c r="M102" s="35"/>
+      <c r="N102" s="35"/>
+      <c r="O102" s="35"/>
+      <c r="P102" s="35"/>
+      <c r="Q102" s="35"/>
+      <c r="R102" s="35"/>
+      <c r="S102" s="35"/>
+      <c r="T102" s="35"/>
+      <c r="U102" s="35"/>
+      <c r="V102" s="35"/>
+      <c r="W102" s="35"/>
+      <c r="X102" s="35"/>
+      <c r="Y102" s="35"/>
+      <c r="Z102" s="35"/>
+      <c r="AA102" s="35"/>
+      <c r="AB102" s="35"/>
     </row>
     <row r="103" spans="9:28" x14ac:dyDescent="0.3">
-      <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
-      <c r="K103" s="36"/>
-      <c r="L103" s="36"/>
-      <c r="M103" s="36"/>
-      <c r="N103" s="36"/>
-      <c r="O103" s="36"/>
-      <c r="P103" s="36"/>
-      <c r="Q103" s="36"/>
-      <c r="R103" s="36"/>
-      <c r="S103" s="36"/>
-      <c r="T103" s="36"/>
-      <c r="U103" s="36"/>
-      <c r="V103" s="36"/>
-      <c r="W103" s="36"/>
-      <c r="X103" s="36"/>
-      <c r="Y103" s="36"/>
-      <c r="Z103" s="36"/>
-      <c r="AA103" s="36"/>
-      <c r="AB103" s="36"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
+      <c r="P103" s="35"/>
+      <c r="Q103" s="35"/>
+      <c r="R103" s="35"/>
+      <c r="S103" s="35"/>
+      <c r="T103" s="35"/>
+      <c r="U103" s="35"/>
+      <c r="V103" s="35"/>
+      <c r="W103" s="35"/>
+      <c r="X103" s="35"/>
+      <c r="Y103" s="35"/>
+      <c r="Z103" s="35"/>
+      <c r="AA103" s="35"/>
+      <c r="AB103" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2894,4 +2966,456 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA75520-D1E6-4FBF-87D5-CF194533B44B}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" customWidth="1"/>
+    <col min="4" max="4" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="2.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="2.44140625" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="2.44140625" customWidth="1"/>
+    <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="2.44140625" customWidth="1"/>
+    <col min="21" max="22" width="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="2.5546875" customWidth="1"/>
+    <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="30" width="2.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W7" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z7" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="R8">
+        <v>15</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V8" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y8">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U9">
+        <v>16</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y9" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z9" s="39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="L10">
+        <v>17</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S10" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V10" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="U12">
+        <v>18</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="V13" s="38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="U14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done 5.Adding Images to your pages, Meeting the Media
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7627DBC8-6AFC-44CA-97AE-EFA8E5266957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811BF60-4D2B-4C56-BD4F-1A0CC8F9D8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12852" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
     <sheet name="4. Getting Connected A Trip to " sheetId="2" r:id="rId2"/>
+    <sheet name="5. Adding Images to your page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="180">
   <si>
     <t>Label</t>
   </si>
@@ -571,13 +572,16 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +631,13 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -862,7 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -942,11 +953,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -963,6 +975,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>11723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>506665</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>13132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D219C284-8652-47B3-AD16-15FBBD6180AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2919046"/>
+          <a:ext cx="5500696" cy="4362394"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>158261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>7919</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>164106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A9A968-7C43-4945-A1BD-74EDD50A04E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7426569"/>
+          <a:ext cx="5611550" cy="4548537"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2168,12 +2273,12 @@
       <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
     </row>
     <row r="58" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
@@ -2972,7 +3077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA75520-D1E6-4FBF-87D5-CF194533B44B}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -3017,13 +3122,13 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>169</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="47" t="s">
         <v>164</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -3034,13 +3139,13 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>160</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="47" t="s">
         <v>165</v>
       </c>
       <c r="N3" s="38" t="s">
@@ -3054,13 +3159,13 @@
       <c r="A4">
         <v>7</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>161</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
         <v>166</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -3086,13 +3191,13 @@
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>162</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="47" t="s">
         <v>167</v>
       </c>
       <c r="J5" s="38" t="s">
@@ -3127,13 +3232,13 @@
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>163</v>
       </c>
       <c r="C6">
         <v>9</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="47" t="s">
         <v>168</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -3171,13 +3276,13 @@
       <c r="A7">
         <v>12</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>170</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="47" t="s">
         <v>175</v>
       </c>
       <c r="P7" s="2" t="s">
@@ -3195,7 +3300,7 @@
       <c r="T7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U7" s="49" t="s">
+      <c r="U7" s="48" t="s">
         <v>38</v>
       </c>
       <c r="V7" s="2" t="s">
@@ -3218,7 +3323,7 @@
       <c r="C8">
         <v>14</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="47" t="s">
         <v>176</v>
       </c>
       <c r="R8">
@@ -3250,13 +3355,13 @@
       <c r="A9">
         <v>16</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>172</v>
       </c>
       <c r="C9">
         <v>15</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="47" t="s">
         <v>177</v>
       </c>
       <c r="I9">
@@ -3303,7 +3408,7 @@
       <c r="A10">
         <v>17</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>173</v>
       </c>
       <c r="L10">
@@ -3341,7 +3446,7 @@
       <c r="A11">
         <v>18</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>174</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -3358,7 +3463,7 @@
       <c r="A12">
         <v>19</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>162</v>
       </c>
       <c r="M12" s="2" t="s">
@@ -3418,4 +3523,367 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E628D8-4704-4EA0-AEFC-4F7B7ED53972}">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="18" width="2.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F5" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F7" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="50">
+        <v>10</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="50">
+        <v>12</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P11" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="50">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed '6. Standards and all that Jazz...'
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811BF60-4D2B-4C56-BD4F-1A0CC8F9D8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C77ED7D-E824-471C-BA39-488A62248CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9612" yWindow="972" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
     <sheet name="4. Getting Connected A Trip to " sheetId="2" r:id="rId2"/>
     <sheet name="5. Adding Images to your page" sheetId="3" r:id="rId3"/>
+    <sheet name="6. Standards and all that Jazz" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="180">
   <si>
     <t>Label</t>
   </si>
@@ -955,10 +956,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2273,12 +2274,12 @@
       <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="49"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
     </row>
     <row r="58" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
@@ -3529,7 +3530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E628D8-4704-4EA0-AEFC-4F7B7ED53972}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
@@ -3752,7 +3753,7 @@
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="49">
         <v>10</v>
       </c>
       <c r="F10" s="38" t="s">
@@ -3778,7 +3779,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="50">
+      <c r="A11" s="49">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3799,7 +3800,7 @@
       <c r="H11" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="50">
+      <c r="K11" s="49">
         <v>12</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -3828,7 +3829,7 @@
       <c r="F12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G12" s="49">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -3851,7 +3852,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="50">
+      <c r="A13" s="49">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3886,4 +3887,354 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86E9816-F86A-4BE1-A33D-F64C2201B381}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="19" width="2.88671875" customWidth="1"/>
+    <col min="20" max="36" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D9" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D11" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H13" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+      <c r="M13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="N15" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed "7. Getting Started with CSS"
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C77ED7D-E824-471C-BA39-488A62248CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F704492-5071-4494-9789-53DB09EF9F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9612" yWindow="972" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
     <sheet name="4. Getting Connected A Trip to " sheetId="2" r:id="rId2"/>
     <sheet name="5. Adding Images to your page" sheetId="3" r:id="rId3"/>
     <sheet name="6. Standards and all that Jazz" sheetId="4" r:id="rId4"/>
+    <sheet name="7. Getting started w CSS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="193">
   <si>
     <t>Label</t>
   </si>
@@ -576,6 +577,45 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a, em</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -874,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -960,6 +1000,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1060,6 +1109,55 @@
         <a:xfrm>
           <a:off x="0" y="7426569"/>
           <a:ext cx="5611550" cy="4548537"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>99848</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>289986</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>46118</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C00F759F-D120-40BC-8D9B-FBDD8EE14948}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="472965" y="1718441"/>
+          <a:ext cx="3921311" cy="2925953"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3893,7 +3991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86E9816-F86A-4BE1-A33D-F64C2201B381}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
@@ -4237,4 +4335,809 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5640DA68-F142-4E83-93A5-A20D6A12FAF9}">
+  <dimension ref="A1:AJ19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AE17" sqref="AE17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="12" width="5.44140625" customWidth="1"/>
+    <col min="14" max="57" width="2.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="F2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="35"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A4" s="35"/>
+      <c r="B4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="I4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49">
+        <v>3</v>
+      </c>
+      <c r="T4" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="49"/>
+      <c r="AH4" s="49"/>
+      <c r="AI4" s="49"/>
+      <c r="AJ4" s="49"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49">
+        <v>6</v>
+      </c>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49">
+        <v>7</v>
+      </c>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD6" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE6" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF6" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG6" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH6" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6" s="49"/>
+      <c r="AJ6" s="49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49">
+        <v>8</v>
+      </c>
+      <c r="V7" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="W7" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="X7" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="49"/>
+      <c r="AC7" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD7" s="49"/>
+      <c r="AE7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF7" s="49"/>
+      <c r="AG7" s="49"/>
+      <c r="AH7" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI7" s="49"/>
+      <c r="AJ7" s="52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="H8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49">
+        <v>10</v>
+      </c>
+      <c r="U9" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="W9" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI9" s="49"/>
+      <c r="AJ9" s="52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49">
+        <v>12</v>
+      </c>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI10" s="49"/>
+      <c r="AJ10" s="52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="R11" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="S11" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="T11" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="U11" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="49">
+        <v>13</v>
+      </c>
+      <c r="W11" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="X11" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y11" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z11" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA11" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="49"/>
+      <c r="AH11" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI11" s="49"/>
+      <c r="AJ11" s="52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI12" s="49"/>
+      <c r="AJ12" s="52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49">
+        <v>14</v>
+      </c>
+      <c r="R13" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="V13" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="W13" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="X13" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y13" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z13" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA13" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI13" s="49"/>
+      <c r="AJ13" s="52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="49"/>
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="49"/>
+      <c r="AC14" s="49"/>
+      <c r="AD14" s="49"/>
+      <c r="AE14" s="49"/>
+      <c r="AF14" s="49"/>
+      <c r="AG14" s="49"/>
+      <c r="AH14" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI14" s="49"/>
+      <c r="AJ14" s="52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49">
+        <v>15</v>
+      </c>
+      <c r="Z15" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA15" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB15" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC15" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD15" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="AE15" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF15" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG15" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH15" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI15" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ15" s="52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="49"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="49"/>
+      <c r="AA16" s="49"/>
+      <c r="AB16" s="49"/>
+      <c r="AC16" s="49"/>
+      <c r="AD16" s="49"/>
+      <c r="AE16" s="49"/>
+      <c r="AF16" s="49"/>
+      <c r="AG16" s="49"/>
+      <c r="AH16" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI16" s="49"/>
+      <c r="AJ16" s="52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="14:36" x14ac:dyDescent="0.3">
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="49"/>
+      <c r="AG17" s="49"/>
+      <c r="AH17" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
+    </row>
+    <row r="18" spans="14:36" x14ac:dyDescent="0.3">
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="49"/>
+      <c r="AA18" s="49"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="49"/>
+      <c r="AD18" s="49"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="49"/>
+      <c r="AG18" s="49"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="49"/>
+      <c r="AJ18" s="49"/>
+    </row>
+    <row r="19" spans="14:36" x14ac:dyDescent="0.3">
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="49"/>
+      <c r="AA19" s="49"/>
+      <c r="AB19" s="49"/>
+      <c r="AC19" s="49"/>
+      <c r="AD19" s="49"/>
+      <c r="AE19" s="49"/>
+      <c r="AF19" s="49"/>
+      <c r="AG19" s="49"/>
+      <c r="AH19" s="49"/>
+      <c r="AI19" s="49"/>
+      <c r="AJ19" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed '9. The box model'
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F704492-5071-4494-9789-53DB09EF9F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87361A00-E082-4299-AAB2-BEEE0D336760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="5. Adding Images to your page" sheetId="3" r:id="rId3"/>
     <sheet name="6. Standards and all that Jazz" sheetId="4" r:id="rId4"/>
     <sheet name="7. Getting started w CSS" sheetId="5" r:id="rId5"/>
+    <sheet name="8. Styling with fonts and color" sheetId="6" r:id="rId6"/>
+    <sheet name="9. The box model" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="197">
   <si>
     <t>Label</t>
   </si>
@@ -616,6 +618,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>e0</t>
+  </si>
+  <si>
+    <t>@</t>
   </si>
 </sst>
 </file>
@@ -914,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -997,9 +1011,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1009,6 +1020,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1438,20 +1457,20 @@
       <selection activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="9" max="28" width="3.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="9" max="28" width="3.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1462,7 +1481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1473,7 +1492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1495,7 +1514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1517,13 +1536,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>149</v>
       </c>
       <c r="B10" s="29"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -1535,7 +1554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1549,7 +1568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1563,7 +1582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1577,7 +1596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1591,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>150</v>
       </c>
@@ -1623,10 +1642,10 @@
       <c r="AA18" s="29"/>
       <c r="AB18" s="29"/>
     </row>
-    <row r="19" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="1" t="s">
@@ -1664,7 +1683,7 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -1688,7 +1707,7 @@
       <c r="AA21" s="5"/>
       <c r="AB21" s="5"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I22" s="1" t="s">
         <v>48</v>
       </c>
@@ -1728,7 +1747,7 @@
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -1752,7 +1771,7 @@
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I24" s="5"/>
       <c r="J24" s="1" t="s">
         <v>36</v>
@@ -1780,7 +1799,7 @@
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I25" s="5"/>
       <c r="J25" s="1" t="s">
         <v>39</v>
@@ -1824,7 +1843,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I26" s="5"/>
       <c r="J26" s="1" t="s">
         <v>43</v>
@@ -1856,7 +1875,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I27" s="5"/>
       <c r="J27" s="1" t="s">
         <v>57</v>
@@ -1888,7 +1907,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="1" t="s">
@@ -1946,7 +1965,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1976,7 +1995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I30" s="5"/>
       <c r="J30" s="1" t="s">
         <v>44</v>
@@ -2008,7 +2027,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I31" s="5"/>
       <c r="J31" s="1" t="s">
         <v>46</v>
@@ -2054,7 +2073,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I32" s="5"/>
       <c r="J32" s="1" t="s">
         <v>47</v>
@@ -2090,7 +2109,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I33" s="5"/>
       <c r="J33" s="1" t="s">
         <v>51</v>
@@ -2124,7 +2143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I34" s="3"/>
       <c r="J34" s="1" t="s">
         <v>46</v>
@@ -2153,7 +2172,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I35" s="3"/>
       <c r="J35" s="1" t="s">
         <v>53</v>
@@ -2184,7 +2203,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="5"/>
       <c r="C36" s="3"/>
@@ -2201,7 +2220,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="5"/>
       <c r="C37" s="3"/>
@@ -2216,7 +2235,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
         <v>151</v>
       </c>
@@ -2233,7 +2252,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>58</v>
@@ -2242,7 +2261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
@@ -2253,7 +2272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>64</v>
       </c>
@@ -2264,7 +2283,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -2275,7 +2294,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -2286,7 +2305,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
@@ -2297,7 +2316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
@@ -2308,7 +2327,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>74</v>
       </c>
@@ -2319,7 +2338,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>76</v>
       </c>
@@ -2330,7 +2349,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>78</v>
       </c>
@@ -2341,7 +2360,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>80</v>
       </c>
@@ -2352,34 +2371,34 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="28" t="s">
         <v>152</v>
       </c>
       <c r="B53" s="32"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="15"/>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="50" t="s">
+    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
-    </row>
-    <row r="58" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+    </row>
+    <row r="58" spans="1:4" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="18" t="s">
         <v>85</v>
       </c>
@@ -2393,7 +2412,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="21"/>
       <c r="B59" s="16" t="s">
         <v>89</v>
@@ -2405,7 +2424,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="23" t="s">
         <v>92</v>
       </c>
@@ -2419,7 +2438,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="21" t="s">
         <v>96</v>
       </c>
@@ -2433,7 +2452,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="23" t="s">
         <v>100</v>
       </c>
@@ -2447,7 +2466,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="21" t="s">
         <v>104</v>
       </c>
@@ -2461,7 +2480,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="23" t="s">
         <v>108</v>
       </c>
@@ -2475,7 +2494,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="21" t="s">
         <v>112</v>
       </c>
@@ -2489,7 +2508,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="23" t="s">
         <v>116</v>
       </c>
@@ -2503,7 +2522,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="21" t="s">
         <v>120</v>
       </c>
@@ -2517,7 +2536,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="23" t="s">
         <v>124</v>
       </c>
@@ -2531,7 +2550,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="21" t="s">
         <v>128</v>
       </c>
@@ -2545,7 +2564,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="25" t="s">
         <v>132</v>
       </c>
@@ -2559,80 +2578,80 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="33"/>
       <c r="B71" s="34"/>
       <c r="C71" s="34"/>
       <c r="D71" s="34"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="28" t="s">
         <v>153</v>
       </c>
       <c r="B73" s="28"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A87" s="28" t="s">
         <v>150</v>
       </c>
       <c r="B87" s="29"/>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I88" s="2">
         <v>1</v>
       </c>
@@ -2666,7 +2685,7 @@
       <c r="AA88" s="35"/>
       <c r="AB88" s="35"/>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I89" s="35"/>
       <c r="J89" s="35"/>
       <c r="K89" s="35"/>
@@ -2696,7 +2715,7 @@
       <c r="AA89" s="35"/>
       <c r="AB89" s="35"/>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I90" s="35"/>
       <c r="J90" s="2" t="s">
         <v>53</v>
@@ -2740,7 +2759,7 @@
       <c r="AA90" s="35"/>
       <c r="AB90" s="35"/>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I91" s="35"/>
       <c r="J91" s="35"/>
       <c r="K91" s="35"/>
@@ -2780,7 +2799,7 @@
       <c r="AA91" s="35"/>
       <c r="AB91" s="35"/>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I92" s="35"/>
       <c r="J92" s="35"/>
       <c r="K92" s="35"/>
@@ -2822,7 +2841,7 @@
       <c r="AA92" s="35"/>
       <c r="AB92" s="35"/>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I93" s="35"/>
       <c r="J93" s="44" t="s">
         <v>51</v>
@@ -2856,7 +2875,7 @@
       <c r="AA93" s="35"/>
       <c r="AB93" s="35"/>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I94" s="35"/>
       <c r="J94" s="44" t="s">
         <v>46</v>
@@ -2900,7 +2919,7 @@
       <c r="AA94" s="35"/>
       <c r="AB94" s="35"/>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I95" s="35"/>
       <c r="J95" s="44" t="s">
         <v>44</v>
@@ -2932,7 +2951,7 @@
       <c r="AA95" s="35"/>
       <c r="AB95" s="35"/>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.35">
       <c r="I96" s="35"/>
       <c r="J96" s="44" t="s">
         <v>45</v>
@@ -2964,7 +2983,7 @@
       <c r="AA96" s="35"/>
       <c r="AB96" s="35"/>
     </row>
-    <row r="97" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="97" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I97" s="35"/>
       <c r="J97" s="44" t="s">
         <v>44</v>
@@ -2996,7 +3015,7 @@
       <c r="AA97" s="35"/>
       <c r="AB97" s="35"/>
     </row>
-    <row r="98" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="98" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I98" s="35"/>
       <c r="J98" s="35"/>
       <c r="K98" s="35"/>
@@ -3024,7 +3043,7 @@
       <c r="AA98" s="35"/>
       <c r="AB98" s="35"/>
     </row>
-    <row r="99" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="99" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I99" s="35"/>
       <c r="J99" s="35"/>
       <c r="K99" s="35"/>
@@ -3072,7 +3091,7 @@
       <c r="AA99" s="35"/>
       <c r="AB99" s="35"/>
     </row>
-    <row r="100" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="100" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I100" s="35"/>
       <c r="J100" s="35"/>
       <c r="K100" s="35"/>
@@ -3094,7 +3113,7 @@
       <c r="AA100" s="35"/>
       <c r="AB100" s="35"/>
     </row>
-    <row r="101" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="101" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I101" s="35"/>
       <c r="J101" s="35"/>
       <c r="K101" s="35"/>
@@ -3116,7 +3135,7 @@
       <c r="AA101" s="35"/>
       <c r="AB101" s="35"/>
     </row>
-    <row r="102" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="102" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I102" s="35"/>
       <c r="J102" s="35"/>
       <c r="K102" s="35"/>
@@ -3138,7 +3157,7 @@
       <c r="AA102" s="35"/>
       <c r="AB102" s="35"/>
     </row>
-    <row r="103" spans="9:28" x14ac:dyDescent="0.3">
+    <row r="103" spans="9:28" x14ac:dyDescent="0.35">
       <c r="I103" s="35"/>
       <c r="J103" s="35"/>
       <c r="K103" s="35"/>
@@ -3180,26 +3199,26 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" customWidth="1"/>
-    <col min="4" max="4" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" customWidth="1"/>
+    <col min="4" max="4" width="56.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="2.453125" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="2.44140625" customWidth="1"/>
+    <col min="10" max="11" width="2.453125" customWidth="1"/>
     <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="2.44140625" customWidth="1"/>
+    <col min="13" max="17" width="2.453125" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="2.44140625" customWidth="1"/>
+    <col min="19" max="20" width="2.453125" customWidth="1"/>
     <col min="21" max="22" width="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="2.5546875" customWidth="1"/>
+    <col min="23" max="24" width="2.54296875" customWidth="1"/>
     <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="30" width="2.5546875" customWidth="1"/>
+    <col min="26" max="30" width="2.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>158</v>
       </c>
@@ -3217,7 +3236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3234,7 +3253,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3254,7 +3273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7</v>
       </c>
@@ -3286,7 +3305,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>8</v>
       </c>
@@ -3327,7 +3346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10</v>
       </c>
@@ -3371,7 +3390,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>12</v>
       </c>
@@ -3412,7 +3431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>13</v>
       </c>
@@ -3450,7 +3469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>16</v>
       </c>
@@ -3503,7 +3522,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>17</v>
       </c>
@@ -3541,7 +3560,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>18</v>
       </c>
@@ -3558,7 +3577,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>19</v>
       </c>
@@ -3590,12 +3609,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="V13" s="38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="U14" s="2" t="s">
         <v>48</v>
       </c>
@@ -3632,17 +3651,17 @@
       <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="2.5546875" customWidth="1"/>
+    <col min="1" max="18" width="2.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C2">
         <v>1</v>
       </c>
@@ -3668,7 +3687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F3" s="2" t="s">
         <v>49</v>
       </c>
@@ -3676,7 +3695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="E4">
         <v>3</v>
       </c>
@@ -3717,7 +3736,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F5" s="38" t="s">
         <v>43</v>
       </c>
@@ -3728,7 +3747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3775,7 +3794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F7" s="41" t="s">
         <v>44</v>
       </c>
@@ -3789,7 +3808,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>8</v>
       </c>
@@ -3830,7 +3849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>9</v>
       </c>
@@ -3847,7 +3866,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>179</v>
       </c>
@@ -3876,7 +3895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="49">
         <v>11</v>
       </c>
@@ -3920,7 +3939,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B12" s="38" t="s">
         <v>43</v>
       </c>
@@ -3949,7 +3968,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="49">
         <v>14</v>
       </c>
@@ -3972,7 +3991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="F14" s="2" t="s">
         <v>50</v>
       </c>
@@ -3995,13 +4014,13 @@
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="19" width="2.88671875" customWidth="1"/>
-    <col min="20" max="36" width="2.6640625" customWidth="1"/>
+    <col min="1" max="19" width="2.90625" customWidth="1"/>
+    <col min="20" max="36" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -4009,7 +4028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4050,7 +4069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" s="2">
         <v>3</v>
       </c>
@@ -4061,7 +4080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
@@ -4072,7 +4091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D5" s="2" t="s">
         <v>154</v>
       </c>
@@ -4098,7 +4117,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
@@ -4109,7 +4128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D7" s="2" t="s">
         <v>43</v>
       </c>
@@ -4117,7 +4136,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
@@ -4149,7 +4168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D9" s="38" t="s">
         <v>154</v>
       </c>
@@ -4163,7 +4182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>8</v>
       </c>
@@ -4201,7 +4220,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D11" s="39" t="s">
         <v>39</v>
       </c>
@@ -4215,7 +4234,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4259,7 +4278,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H13" s="39" t="s">
         <v>39</v>
       </c>
@@ -4276,7 +4295,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J14" s="2" t="s">
         <v>47</v>
       </c>
@@ -4287,7 +4306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H15">
         <v>14</v>
       </c>
@@ -4313,7 +4332,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J16" s="2" t="s">
         <v>48</v>
       </c>
@@ -4324,7 +4343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J17" s="2" t="s">
         <v>50</v>
       </c>
@@ -4341,17 +4360,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5640DA68-F142-4E83-93A5-A20D6A12FAF9}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="AE17" sqref="AE17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="12" width="5.44140625" customWidth="1"/>
-    <col min="14" max="57" width="2.77734375" customWidth="1"/>
+    <col min="1" max="12" width="5.453125" customWidth="1"/>
+    <col min="14" max="57" width="2.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="N1" s="49"/>
       <c r="O1" s="49"/>
       <c r="P1" s="49"/>
@@ -4376,7 +4395,7 @@
       <c r="AI1" s="49"/>
       <c r="AJ1" s="49"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="35"/>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -4411,9 +4430,9 @@
       <c r="AI2" s="49"/>
       <c r="AJ2" s="49"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="35"/>
       <c r="N3" s="49"/>
       <c r="O3" s="49"/>
@@ -4430,11 +4449,11 @@
       </c>
       <c r="Y3" s="49"/>
       <c r="Z3" s="49"/>
-      <c r="AA3" s="52" t="s">
+      <c r="AA3" s="51" t="s">
         <v>44</v>
       </c>
       <c r="AB3" s="49"/>
-      <c r="AC3" s="52" t="s">
+      <c r="AC3" s="51" t="s">
         <v>44</v>
       </c>
       <c r="AD3" s="49"/>
@@ -4445,7 +4464,7 @@
       <c r="AI3" s="49"/>
       <c r="AJ3" s="49"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="35"/>
       <c r="B4" s="2" t="s">
         <v>182</v>
@@ -4462,28 +4481,28 @@
       <c r="S4" s="49">
         <v>3</v>
       </c>
-      <c r="T4" s="52" t="s">
+      <c r="T4" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="U4" s="52" t="s">
+      <c r="U4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="V4" s="52" t="s">
+      <c r="V4" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="52" t="s">
+      <c r="W4" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4" s="51" t="s">
         <v>44</v>
       </c>
       <c r="Y4" s="49"/>
       <c r="Z4" s="49"/>
-      <c r="AA4" s="52" t="s">
+      <c r="AA4" s="51" t="s">
         <v>38</v>
       </c>
       <c r="AB4" s="49"/>
-      <c r="AC4" s="52" t="s">
+      <c r="AC4" s="51" t="s">
         <v>45</v>
       </c>
       <c r="AD4" s="49"/>
@@ -4494,7 +4513,7 @@
       <c r="AI4" s="49"/>
       <c r="AJ4" s="49"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -4508,16 +4527,16 @@
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
-      <c r="X5" s="52" t="s">
+      <c r="X5" s="51" t="s">
         <v>45</v>
       </c>
       <c r="Y5" s="49"/>
       <c r="Z5" s="49"/>
-      <c r="AA5" s="54" t="s">
+      <c r="AA5" s="53" t="s">
         <v>53</v>
       </c>
       <c r="AB5" s="49"/>
-      <c r="AC5" s="52" t="s">
+      <c r="AC5" s="51" t="s">
         <v>50</v>
       </c>
       <c r="AD5" s="49"/>
@@ -4532,7 +4551,7 @@
       <c r="AI5" s="49"/>
       <c r="AJ5" s="49"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>183</v>
       </c>
@@ -4567,33 +4586,33 @@
       <c r="U6" s="49"/>
       <c r="V6" s="49"/>
       <c r="W6" s="49"/>
-      <c r="X6" s="54" t="s">
+      <c r="X6" s="53" t="s">
         <v>50</v>
       </c>
       <c r="Y6" s="49"/>
       <c r="Z6" s="49"/>
-      <c r="AA6" s="52" t="s">
+      <c r="AA6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="AB6" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC6" s="52" t="s">
+      <c r="AB6" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="AD6" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE6" s="52" t="s">
+      <c r="AD6" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE6" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AF6" s="57" t="s">
+      <c r="AF6" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="AG6" s="53" t="s">
+      <c r="AG6" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="AH6" s="52" t="s">
+      <c r="AH6" s="51" t="s">
         <v>39</v>
       </c>
       <c r="AI6" s="49"/>
@@ -4601,7 +4620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="35"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -4615,43 +4634,43 @@
       <c r="U7" s="49">
         <v>8</v>
       </c>
-      <c r="V7" s="52" t="s">
+      <c r="V7" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="W7" s="52" t="s">
+      <c r="W7" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="52" t="s">
+      <c r="X7" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="Y7" s="52" t="s">
+      <c r="Y7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="Z7" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA7" s="56" t="s">
+      <c r="Z7" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA7" s="55" t="s">
         <v>44</v>
       </c>
       <c r="AB7" s="49"/>
-      <c r="AC7" s="52" t="s">
+      <c r="AC7" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AD7" s="49"/>
-      <c r="AE7" s="52" t="s">
+      <c r="AE7" s="51" t="s">
         <v>36</v>
       </c>
       <c r="AF7" s="49"/>
       <c r="AG7" s="49"/>
-      <c r="AH7" s="52" t="s">
+      <c r="AH7" s="51" t="s">
         <v>38</v>
       </c>
       <c r="AI7" s="49"/>
-      <c r="AJ7" s="52" t="s">
+      <c r="AJ7" s="51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
@@ -4677,31 +4696,31 @@
       <c r="U8" s="49"/>
       <c r="V8" s="49"/>
       <c r="W8" s="49"/>
-      <c r="X8" s="55" t="s">
+      <c r="X8" s="54" t="s">
         <v>43</v>
       </c>
       <c r="Y8" s="49"/>
       <c r="Z8" s="49"/>
-      <c r="AA8" s="52" t="s">
+      <c r="AA8" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AB8" s="49"/>
       <c r="AC8" s="49"/>
       <c r="AD8" s="49"/>
-      <c r="AE8" s="52" t="s">
+      <c r="AE8" s="51" t="s">
         <v>46</v>
       </c>
       <c r="AF8" s="49"/>
       <c r="AG8" s="49"/>
-      <c r="AH8" s="52" t="s">
+      <c r="AH8" s="51" t="s">
         <v>48</v>
       </c>
       <c r="AI8" s="49"/>
-      <c r="AJ8" s="52" t="s">
+      <c r="AJ8" s="51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="35"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -4714,42 +4733,42 @@
       <c r="T9" s="49">
         <v>10</v>
       </c>
-      <c r="U9" s="52" t="s">
+      <c r="U9" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="V9" s="52" t="s">
+      <c r="V9" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="52" t="s">
+      <c r="W9" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="X9" s="52" t="s">
+      <c r="X9" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="Y9" s="52" t="s">
+      <c r="Y9" s="51" t="s">
         <v>44</v>
       </c>
       <c r="Z9" s="49"/>
-      <c r="AA9" s="52" t="s">
+      <c r="AA9" s="51" t="s">
         <v>39</v>
       </c>
       <c r="AB9" s="49"/>
       <c r="AC9" s="49"/>
       <c r="AD9" s="49"/>
-      <c r="AE9" s="52" t="s">
+      <c r="AE9" s="51" t="s">
         <v>51</v>
       </c>
       <c r="AF9" s="49"/>
       <c r="AG9" s="49"/>
-      <c r="AH9" s="52" t="s">
+      <c r="AH9" s="51" t="s">
         <v>154</v>
       </c>
       <c r="AI9" s="49"/>
-      <c r="AJ9" s="52" t="s">
+      <c r="AJ9" s="51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -4765,31 +4784,31 @@
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49"/>
-      <c r="X10" s="55" t="s">
+      <c r="X10" s="54" t="s">
         <v>36</v>
       </c>
       <c r="Y10" s="49"/>
       <c r="Z10" s="49"/>
-      <c r="AA10" s="52" t="s">
+      <c r="AA10" s="51" t="s">
         <v>46</v>
       </c>
       <c r="AB10" s="49"/>
       <c r="AC10" s="49"/>
       <c r="AD10" s="49"/>
-      <c r="AE10" s="52" t="s">
+      <c r="AE10" s="51" t="s">
         <v>48</v>
       </c>
       <c r="AF10" s="49"/>
       <c r="AG10" s="49"/>
-      <c r="AH10" s="52" t="s">
+      <c r="AH10" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AI10" s="49"/>
-      <c r="AJ10" s="52" t="s">
+      <c r="AJ10" s="51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="35"/>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
@@ -4798,56 +4817,56 @@
       <c r="P11" s="49">
         <v>11</v>
       </c>
-      <c r="Q11" s="52" t="s">
+      <c r="Q11" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="R11" s="52" t="s">
+      <c r="R11" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="S11" s="52" t="s">
+      <c r="S11" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="T11" s="52" t="s">
+      <c r="T11" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="U11" s="52" t="s">
+      <c r="U11" s="51" t="s">
         <v>39</v>
       </c>
       <c r="V11" s="49">
         <v>13</v>
       </c>
-      <c r="W11" s="52" t="s">
+      <c r="W11" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="X11" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y11" s="52" t="s">
+      <c r="X11" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y11" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="Z11" s="53" t="s">
+      <c r="Z11" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="AA11" s="52" t="s">
+      <c r="AA11" s="51" t="s">
         <v>57</v>
       </c>
       <c r="AB11" s="49"/>
       <c r="AC11" s="49"/>
       <c r="AD11" s="49"/>
-      <c r="AE11" s="52" t="s">
+      <c r="AE11" s="51" t="s">
         <v>39</v>
       </c>
       <c r="AF11" s="49"/>
       <c r="AG11" s="49"/>
-      <c r="AH11" s="52" t="s">
+      <c r="AH11" s="51" t="s">
         <v>47</v>
       </c>
       <c r="AI11" s="49"/>
-      <c r="AJ11" s="52" t="s">
+      <c r="AJ11" s="51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -4856,14 +4875,14 @@
       <c r="P12" s="49"/>
       <c r="Q12" s="49"/>
       <c r="R12" s="49"/>
-      <c r="S12" s="56" t="s">
+      <c r="S12" s="55" t="s">
         <v>46</v>
       </c>
       <c r="T12" s="49"/>
       <c r="U12" s="49"/>
       <c r="V12" s="49"/>
       <c r="W12" s="49"/>
-      <c r="X12" s="55" t="s">
+      <c r="X12" s="54" t="s">
         <v>43</v>
       </c>
       <c r="Y12" s="49"/>
@@ -4872,20 +4891,20 @@
       <c r="AB12" s="49"/>
       <c r="AC12" s="49"/>
       <c r="AD12" s="49"/>
-      <c r="AE12" s="52" t="s">
+      <c r="AE12" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AF12" s="49"/>
       <c r="AG12" s="49"/>
-      <c r="AH12" s="52" t="s">
+      <c r="AH12" s="51" t="s">
         <v>48</v>
       </c>
       <c r="AI12" s="49"/>
-      <c r="AJ12" s="52" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AJ12" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -4895,55 +4914,55 @@
       <c r="Q13" s="49">
         <v>14</v>
       </c>
-      <c r="R13" s="53" t="s">
+      <c r="R13" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="S13" s="52" t="s">
+      <c r="S13" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="T13" s="57" t="s">
+      <c r="T13" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="U13" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="V13" s="52" t="s">
+      <c r="U13" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="V13" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="W13" s="52" t="s">
+      <c r="W13" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="X13" s="52" t="s">
+      <c r="X13" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="Y13" s="52" t="s">
+      <c r="Y13" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="Z13" s="52" t="s">
+      <c r="Z13" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="AA13" s="52" t="s">
+      <c r="AA13" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AB13" s="52" t="s">
+      <c r="AB13" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AC13" s="49"/>
       <c r="AD13" s="49"/>
-      <c r="AE13" s="52" t="s">
+      <c r="AE13" s="51" t="s">
         <v>53</v>
       </c>
       <c r="AF13" s="49"/>
       <c r="AG13" s="49"/>
-      <c r="AH13" s="52" t="s">
+      <c r="AH13" s="51" t="s">
         <v>43</v>
       </c>
       <c r="AI13" s="49"/>
-      <c r="AJ13" s="52" t="s">
+      <c r="AJ13" s="51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="35"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -4952,7 +4971,7 @@
       <c r="P14" s="49"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="49"/>
-      <c r="S14" s="52" t="s">
+      <c r="S14" s="51" t="s">
         <v>40</v>
       </c>
       <c r="T14" s="49"/>
@@ -4969,15 +4988,15 @@
       <c r="AE14" s="49"/>
       <c r="AF14" s="49"/>
       <c r="AG14" s="49"/>
-      <c r="AH14" s="54" t="s">
+      <c r="AH14" s="53" t="s">
         <v>44</v>
       </c>
       <c r="AI14" s="49"/>
-      <c r="AJ14" s="52" t="s">
+      <c r="AJ14" s="51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
@@ -4995,41 +5014,41 @@
       <c r="Y15" s="49">
         <v>15</v>
       </c>
-      <c r="Z15" s="52" t="s">
+      <c r="Z15" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="AA15" s="52" t="s">
+      <c r="AA15" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="AB15" s="52" t="s">
+      <c r="AB15" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="AC15" s="52" t="s">
+      <c r="AC15" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="AD15" s="59" t="s">
+      <c r="AD15" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="AE15" s="52" t="s">
+      <c r="AE15" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="AF15" s="52" t="s">
+      <c r="AF15" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="AG15" s="52" t="s">
+      <c r="AG15" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="AH15" s="52" t="s">
+      <c r="AH15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="AI15" s="53" t="s">
+      <c r="AI15" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="AJ15" s="52" t="s">
+      <c r="AJ15" s="51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="N16" s="49"/>
       <c r="O16" s="49"/>
       <c r="P16" s="49"/>
@@ -5050,15 +5069,15 @@
       <c r="AE16" s="49"/>
       <c r="AF16" s="49"/>
       <c r="AG16" s="49"/>
-      <c r="AH16" s="56" t="s">
+      <c r="AH16" s="55" t="s">
         <v>54</v>
       </c>
       <c r="AI16" s="49"/>
-      <c r="AJ16" s="52" t="s">
+      <c r="AJ16" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="14:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="14:36" x14ac:dyDescent="0.35">
       <c r="N17" s="49"/>
       <c r="O17" s="49"/>
       <c r="P17" s="49"/>
@@ -5079,13 +5098,13 @@
       <c r="AE17" s="49"/>
       <c r="AF17" s="49"/>
       <c r="AG17" s="49"/>
-      <c r="AH17" s="52" t="s">
+      <c r="AH17" s="51" t="s">
         <v>53</v>
       </c>
       <c r="AI17" s="49"/>
       <c r="AJ17" s="49"/>
     </row>
-    <row r="18" spans="14:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="14:36" x14ac:dyDescent="0.35">
       <c r="N18" s="49"/>
       <c r="O18" s="49"/>
       <c r="P18" s="49"/>
@@ -5110,7 +5129,7 @@
       <c r="AI18" s="49"/>
       <c r="AJ18" s="49"/>
     </row>
-    <row r="19" spans="14:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="14:36" x14ac:dyDescent="0.35">
       <c r="N19" s="49"/>
       <c r="O19" s="49"/>
       <c r="P19" s="49"/>
@@ -5140,4 +5159,967 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2955917-9A2D-463B-9C32-52C7D8FDE766}">
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="45" width="3.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="59">
+        <v>17</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>8 + 16*11</f>
+        <v>184</v>
+      </c>
+      <c r="C3">
+        <f>7 + 16*1</f>
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <f>0 + 14*16</f>
+        <v>224</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="U5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="N7" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L9" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L11" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S14" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I15" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="14:18" x14ac:dyDescent="0.35">
+      <c r="N17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE4D602-FB80-44B3-A50C-2E59D60B4E34}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="39" width="3.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="Q1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35">
+        <v>3</v>
+      </c>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35">
+        <v>6</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35">
+        <v>7</v>
+      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35">
+        <v>8</v>
+      </c>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="35"/>
+      <c r="M9" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="S9" s="38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F10" s="35"/>
+      <c r="G10" s="35">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35">
+        <v>10</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="35"/>
+      <c r="M11" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35">
+        <v>11</v>
+      </c>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="S11" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="35"/>
+      <c r="O12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="S12" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="35">
+        <v>13</v>
+      </c>
+      <c r="M13" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T13" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="35"/>
+      <c r="M14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="35"/>
+      <c r="O14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="U14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="35"/>
+      <c r="M15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="35"/>
+      <c r="O15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="U15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35">
+        <v>14</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17" x14ac:dyDescent="0.35">
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.35">
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.35">
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.35">
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+    </row>
+    <row r="21" spans="6:17" x14ac:dyDescent="0.35">
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed '11.Layout and positioning - Arranging Elements'
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\HTML_CSS\Head_First_HTML_CSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87361A00-E082-4299-AAB2-BEEE0D336760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBFE983-F35A-49F4-A8A5-99849A3B2C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3. Building Blocks Web Page C" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="7. Getting started w CSS" sheetId="5" r:id="rId5"/>
     <sheet name="8. Styling with fonts and color" sheetId="6" r:id="rId6"/>
     <sheet name="9. The box model" sheetId="7" r:id="rId7"/>
+    <sheet name="11. Arranging Elements" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="197">
   <si>
     <t>Label</t>
   </si>
@@ -636,7 +637,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +690,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -928,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1024,10 +1039,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2391,12 +2417,12 @@
       <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="61" t="s">
+      <c r="A57" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="61"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
     </row>
     <row r="58" spans="1:4" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="18" t="s">
@@ -5586,7 +5612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE4D602-FB80-44B3-A50C-2E59D60B4E34}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
@@ -5997,7 +6023,7 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="F15" s="35"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="62"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
       <c r="K15" s="2" t="s">
@@ -6122,4 +6148,1063 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830EAE1D-20DA-4BD5-B389-108182E443F6}">
+  <dimension ref="A1:AJ24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="39" width="3.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63">
+        <v>1</v>
+      </c>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63">
+        <v>2</v>
+      </c>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AG2" s="64"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63">
+        <v>3</v>
+      </c>
+      <c r="L3" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63">
+        <v>5</v>
+      </c>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="67"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F4" s="64"/>
+      <c r="G4" s="63">
+        <v>6</v>
+      </c>
+      <c r="H4" s="63"/>
+      <c r="I4" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="63">
+        <v>4</v>
+      </c>
+      <c r="K4" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F5" s="64">
+        <v>6</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" s="63"/>
+      <c r="L5" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="67"/>
+      <c r="AI5" s="67"/>
+      <c r="AJ5" s="67"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F6" s="64"/>
+      <c r="G6" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="63"/>
+      <c r="I6" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63">
+        <v>8</v>
+      </c>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63">
+        <v>9</v>
+      </c>
+      <c r="U6" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="64"/>
+      <c r="AD6" s="64"/>
+      <c r="AE6" s="64"/>
+      <c r="AF6" s="64"/>
+      <c r="AG6" s="64"/>
+      <c r="AH6" s="67"/>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F7" s="64"/>
+      <c r="G7" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="63"/>
+      <c r="I7" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63">
+        <v>7</v>
+      </c>
+      <c r="N7" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="64"/>
+      <c r="AC7" s="64"/>
+      <c r="AD7" s="64"/>
+      <c r="AE7" s="64"/>
+      <c r="AF7" s="64"/>
+      <c r="AG7" s="64"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F8" s="64"/>
+      <c r="G8" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="I8" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="63">
+        <v>10</v>
+      </c>
+      <c r="T8" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="U8" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
+      <c r="X8" s="63"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="64"/>
+      <c r="AD8" s="64"/>
+      <c r="AE8" s="64"/>
+      <c r="AF8" s="64"/>
+      <c r="AG8" s="64"/>
+      <c r="AH8" s="67"/>
+      <c r="AI8" s="67"/>
+      <c r="AJ8" s="67"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F9" s="64"/>
+      <c r="G9" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="63">
+        <v>11</v>
+      </c>
+      <c r="I9" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" s="63"/>
+      <c r="T9" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="64"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="64"/>
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="64"/>
+      <c r="AF9" s="64"/>
+      <c r="AG9" s="64"/>
+      <c r="AH9" s="67"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="67"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" s="63"/>
+      <c r="T10" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="64"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64"/>
+      <c r="AD10" s="64"/>
+      <c r="AE10" s="64"/>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63">
+        <v>13</v>
+      </c>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63">
+        <v>12</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="63"/>
+      <c r="T11" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" s="63"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="63"/>
+      <c r="X11" s="63"/>
+      <c r="Y11" s="64"/>
+      <c r="Z11" s="64"/>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="64"/>
+      <c r="AC11" s="64"/>
+      <c r="AD11" s="64"/>
+      <c r="AE11" s="64"/>
+      <c r="AF11" s="64"/>
+      <c r="AG11" s="64"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="63"/>
+      <c r="T12" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" s="63"/>
+      <c r="V12" s="63">
+        <v>14</v>
+      </c>
+      <c r="W12" s="63"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="64"/>
+      <c r="Z12" s="64"/>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="64"/>
+      <c r="AC12" s="64"/>
+      <c r="AD12" s="64"/>
+      <c r="AE12" s="64"/>
+      <c r="AF12" s="64"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="67"/>
+      <c r="AJ12" s="67"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="63"/>
+      <c r="T13" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" s="63"/>
+      <c r="V13" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="64"/>
+      <c r="Z13" s="64"/>
+      <c r="AA13" s="64"/>
+      <c r="AB13" s="64"/>
+      <c r="AC13" s="64"/>
+      <c r="AD13" s="64"/>
+      <c r="AE13" s="64"/>
+      <c r="AF13" s="64"/>
+      <c r="AG13" s="64"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="67"/>
+      <c r="AJ13" s="67"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F14" s="63">
+        <v>15</v>
+      </c>
+      <c r="G14" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="63"/>
+      <c r="T14" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="63"/>
+      <c r="V14" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="W14" s="63"/>
+      <c r="X14" s="63"/>
+      <c r="Y14" s="64"/>
+      <c r="Z14" s="64"/>
+      <c r="AA14" s="64"/>
+      <c r="AB14" s="64"/>
+      <c r="AC14" s="64"/>
+      <c r="AD14" s="64"/>
+      <c r="AE14" s="64"/>
+      <c r="AF14" s="64"/>
+      <c r="AG14" s="64"/>
+      <c r="AH14" s="67"/>
+      <c r="AI14" s="67"/>
+      <c r="AJ14" s="67"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="W15" s="63"/>
+      <c r="X15" s="63"/>
+      <c r="Y15" s="64"/>
+      <c r="Z15" s="64"/>
+      <c r="AA15" s="64"/>
+      <c r="AB15" s="64"/>
+      <c r="AC15" s="64"/>
+      <c r="AD15" s="64"/>
+      <c r="AE15" s="64"/>
+      <c r="AF15" s="64"/>
+      <c r="AG15" s="64"/>
+      <c r="AH15" s="67"/>
+      <c r="AI15" s="67"/>
+      <c r="AJ15" s="67"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
+      <c r="Y16" s="64"/>
+      <c r="Z16" s="64"/>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="64"/>
+      <c r="AD16" s="64"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="64"/>
+      <c r="AG16" s="64"/>
+      <c r="AH16" s="67"/>
+      <c r="AI16" s="67"/>
+      <c r="AJ16" s="67"/>
+    </row>
+    <row r="17" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F17" s="63">
+        <v>16</v>
+      </c>
+      <c r="G17" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63">
+        <v>17</v>
+      </c>
+      <c r="O17" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="R17" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="U17" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="V17" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="W17" s="63"/>
+      <c r="X17" s="63"/>
+      <c r="Y17" s="64"/>
+      <c r="Z17" s="64"/>
+      <c r="AA17" s="64"/>
+      <c r="AB17" s="64"/>
+      <c r="AC17" s="64"/>
+      <c r="AD17" s="64"/>
+      <c r="AE17" s="64"/>
+      <c r="AF17" s="64"/>
+      <c r="AG17" s="64"/>
+      <c r="AH17" s="67"/>
+      <c r="AI17" s="67"/>
+      <c r="AJ17" s="67"/>
+    </row>
+    <row r="18" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
+      <c r="U18" s="63"/>
+      <c r="V18" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="W18" s="63"/>
+      <c r="X18" s="63"/>
+      <c r="Y18" s="64"/>
+      <c r="Z18" s="64"/>
+      <c r="AA18" s="64"/>
+      <c r="AB18" s="64"/>
+      <c r="AC18" s="64"/>
+      <c r="AD18" s="64"/>
+      <c r="AE18" s="64"/>
+      <c r="AF18" s="64"/>
+      <c r="AG18" s="64"/>
+      <c r="AH18" s="67"/>
+      <c r="AI18" s="67"/>
+      <c r="AJ18" s="67"/>
+    </row>
+    <row r="19" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="64"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="63"/>
+      <c r="U19" s="63"/>
+      <c r="V19" s="63"/>
+      <c r="W19" s="63"/>
+      <c r="X19" s="63"/>
+      <c r="Y19" s="64"/>
+      <c r="Z19" s="64"/>
+      <c r="AA19" s="64"/>
+      <c r="AB19" s="64"/>
+      <c r="AC19" s="64"/>
+      <c r="AD19" s="64"/>
+      <c r="AE19" s="64"/>
+      <c r="AF19" s="64"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="67"/>
+      <c r="AI19" s="67"/>
+      <c r="AJ19" s="67"/>
+    </row>
+    <row r="20" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="64"/>
+      <c r="S20" s="64"/>
+      <c r="T20" s="64"/>
+      <c r="U20" s="64"/>
+      <c r="V20" s="64"/>
+      <c r="W20" s="64"/>
+      <c r="X20" s="64"/>
+      <c r="Y20" s="64"/>
+      <c r="Z20" s="64"/>
+      <c r="AA20" s="64"/>
+      <c r="AB20" s="64"/>
+      <c r="AC20" s="64"/>
+      <c r="AD20" s="64"/>
+      <c r="AE20" s="64"/>
+      <c r="AF20" s="64"/>
+      <c r="AG20" s="64"/>
+      <c r="AH20" s="67"/>
+      <c r="AI20" s="67"/>
+      <c r="AJ20" s="67"/>
+    </row>
+    <row r="21" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="64"/>
+      <c r="S21" s="64"/>
+      <c r="T21" s="64"/>
+      <c r="U21" s="64"/>
+      <c r="V21" s="64"/>
+      <c r="W21" s="64"/>
+      <c r="X21" s="64"/>
+      <c r="Y21" s="64"/>
+      <c r="Z21" s="64"/>
+      <c r="AA21" s="64"/>
+      <c r="AB21" s="64"/>
+      <c r="AC21" s="64"/>
+      <c r="AD21" s="64"/>
+      <c r="AE21" s="64"/>
+      <c r="AF21" s="64"/>
+      <c r="AG21" s="64"/>
+      <c r="AH21" s="67"/>
+      <c r="AI21" s="67"/>
+      <c r="AJ21" s="67"/>
+    </row>
+    <row r="22" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="64"/>
+      <c r="S22" s="64"/>
+      <c r="T22" s="64"/>
+      <c r="U22" s="64"/>
+      <c r="V22" s="64"/>
+      <c r="W22" s="64"/>
+      <c r="X22" s="64"/>
+      <c r="Y22" s="64"/>
+      <c r="Z22" s="64"/>
+      <c r="AA22" s="64"/>
+      <c r="AB22" s="64"/>
+      <c r="AC22" s="64"/>
+      <c r="AD22" s="64"/>
+      <c r="AE22" s="64"/>
+      <c r="AF22" s="64"/>
+      <c r="AG22" s="64"/>
+      <c r="AH22" s="67"/>
+      <c r="AI22" s="67"/>
+      <c r="AJ22" s="67"/>
+    </row>
+    <row r="23" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+      <c r="T23" s="67"/>
+      <c r="U23" s="67"/>
+      <c r="V23" s="67"/>
+      <c r="W23" s="67"/>
+      <c r="X23" s="67"/>
+      <c r="Y23" s="67"/>
+      <c r="Z23" s="67"/>
+      <c r="AA23" s="67"/>
+      <c r="AB23" s="67"/>
+      <c r="AC23" s="67"/>
+      <c r="AD23" s="67"/>
+      <c r="AE23" s="67"/>
+      <c r="AF23" s="67"/>
+      <c r="AG23" s="67"/>
+      <c r="AH23" s="67"/>
+      <c r="AI23" s="67"/>
+      <c r="AJ23" s="67"/>
+    </row>
+    <row r="24" spans="6:36" x14ac:dyDescent="0.35">
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
+      <c r="P24" s="67"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="67"/>
+      <c r="U24" s="67"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="67"/>
+      <c r="X24" s="67"/>
+      <c r="Y24" s="67"/>
+      <c r="Z24" s="67"/>
+      <c r="AA24" s="67"/>
+      <c r="AB24" s="67"/>
+      <c r="AC24" s="67"/>
+      <c r="AD24" s="67"/>
+      <c r="AE24" s="67"/>
+      <c r="AF24" s="67"/>
+      <c r="AG24" s="67"/>
+      <c r="AH24" s="67"/>
+      <c r="AI24" s="67"/>
+      <c r="AJ24" s="67"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>